<commit_message>
initial commit - updated report qmd and diary
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookd/teaching/ETC5521/eda-private/assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashvi\Documents\Monash\2023 Sem2\ETC5521\Assignments\assignment-3-peaches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E6E8D6-D05B-C146-B3DA-2457C8448439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2A7E1A-77AA-40B3-B2AF-FE74E6A458FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="820" windowWidth="27860" windowHeight="16940" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Team Name:</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Discussions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fill in as needed </t>
   </si>
   <si>
     <t>eg.
@@ -72,12 +69,33 @@
 Fix merge conflict 
 Decide on choice of methods for first part</t>
   </si>
+  <si>
+    <t>Peaches</t>
+  </si>
+  <si>
+    <t>Tanish</t>
+  </si>
+  <si>
+    <t>Ashvin</t>
+  </si>
+  <si>
+    <t>aran0026</t>
+  </si>
+  <si>
+    <t>tjoh0028</t>
+  </si>
+  <si>
+    <t>1. Decided on the 'wild thing'/animal.
+2. Downloaded and saved the data.     
+3. Set up a plan for the week.
+4. Discusses some things to always consider when working collaboratively on git.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,14 +118,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -129,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -141,7 +151,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,35 +474,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.75" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -496,14 +530,14 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45183</v>
       </c>
@@ -513,16 +547,28 @@
       <c r="C7" s="3">
         <v>0.79861111111111116</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>45187</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minutes logs added and way forward finalised
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rinbaruah/Monash Business School Local/Master of Business Analytics  /Exploratory Data Analysis/Assignments/Assignment 3 Part B/assignment-3-peaches/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rinbaruah/Monash Business School Local/Master of Business Analytics  /Exploratory Data Analysis/Assignments/Assignment 3/Part B/assignment-3-peaches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20940508-ADB2-1C41-A4E7-8B081479CED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF94471-F51C-F04A-8F65-800D06B57997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20700" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Part A" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Team Name:</t>
   </si>
@@ -121,7 +121,10 @@
     <t>abar0090</t>
   </si>
   <si>
-    <t>Initial discussions and way forward</t>
+    <t>3:30 OM</t>
+  </si>
+  <si>
+    <t>Initial discussions and way forward. Tourism data added. Clarifications regarding the data.</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -236,9 +239,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -247,8 +247,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,12 +707,12 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -718,7 +728,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,34 +787,37 @@
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>45213</v>
       </c>
       <c r="B7" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
+      <c r="E7" s="18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generative script AI and meeting logs updated
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kelly/Desktop/ETC5521 - Exploratory Data Analysis/Assignments/Assignment4/assignment-3-peaches/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rinbaruah/Monash Business School Local/Master of Business Analytics  /Exploratory Data Analysis/Assignments/Assignment 3/Part B/assignment-3-peaches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6801B450-0BD7-B840-9E27-AB3C6B032F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D073771-980F-F440-B5D6-2671BB4A318E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Team Name:</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>Fixing previous report expectations, continuing to work on temporal analysis, adding replacing and image</t>
+  </si>
+  <si>
+    <t>Working on report readiness, removing redundant plots, finalised temporal and eco tourism analysis and improved overall report coherency</t>
+  </si>
+  <si>
+    <t>Corected aspects of the heatmap, made all the plot themes uniform, allocated sections for the presentation</t>
+  </si>
+  <si>
+    <t>All + Paired presentation team</t>
+  </si>
+  <si>
+    <t>Presented report, participated in QnA</t>
   </si>
 </sst>
 </file>
@@ -292,12 +304,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6EF314-C21A-2C43-85A5-178F4687F07E}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,17 +922,68 @@
       <c r="A11" s="15">
         <v>45223</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="17" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+      <c r="A12" s="20">
+        <v>45224</v>
+      </c>
+      <c r="B12" s="21">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C12" s="21">
+        <v>0.875</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="20">
+        <v>45225</v>
+      </c>
+      <c r="B13" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="C13" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="20">
+        <v>45225</v>
+      </c>
+      <c r="B14" s="21">
+        <v>0.875</v>
+      </c>
+      <c r="C14" s="21">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>